<commit_message>
Created data missingness folder within data folder and spreadsheet within this folder; completed spreadsheet
</commit_message>
<xml_diff>
--- a/data/data_missingness/Data Missingness.xlsx
+++ b/data/data_missingness/Data Missingness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellameltzer/Git/tropical_cyclones_educational_attainment_2022/data/data_missingness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A86799D0-F051-C043-A518-196BCF78CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1795EA6A-0532-BE49-AA82-126CDD8C671E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{2F47A456-5783-944A-AE3E-11E08F327DC9}"/>
+    <workbookView xWindow="11560" yWindow="500" windowWidth="28040" windowHeight="16240" xr2:uid="{2F47A456-5783-944A-AE3E-11E08F327DC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>State</t>
   </si>
@@ -44,10 +44,70 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Grade</t>
-  </si>
-  <si>
     <t>Year(s)</t>
+  </si>
+  <si>
+    <t>FIPS</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>2009-2010</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Grade(s)</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>RLA</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>2013-2018</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>6, 7, 8</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Revisit x-axis; ends in 2014</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>7, 8</t>
+  </si>
+  <si>
+    <t>2012-2018</t>
+  </si>
+  <si>
+    <t>5, 6, 7, 8</t>
+  </si>
+  <si>
+    <t>2009-2018</t>
+  </si>
+  <si>
+    <t>Revisit x-axis</t>
+  </si>
+  <si>
+    <t>Virginia</t>
   </si>
 </sst>
 </file>
@@ -408,26 +468,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78622C2-A92C-3B46-9DC4-7F5924FFD6AA}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>2014</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>2014</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>